<commit_message>
Dodanie operacji na obrazach
</commit_message>
<xml_diff>
--- a/Badania.xlsx
+++ b/Badania.xlsx
@@ -7,11 +7,8 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="BadaniaWatki" sheetId="4" r:id="rId4"/>
-    <sheet name="BadaniaPararelle" sheetId="5" r:id="rId5"/>
+    <sheet name="BadaniaWatki" sheetId="1" r:id="rId1"/>
+    <sheet name="BadaniaPararelle" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr fullCalcOnLoad="1"/>
@@ -22,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="11">
   <si>
     <t>100x100</t>
   </si>
@@ -46,24 +43,6 @@
   </si>
   <si>
     <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
   </si>
   <si>
     <t>200x200</t>
@@ -530,12 +509,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.28125" widthPt="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="2.28125" widthPt="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="12.75">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" ht="12.75">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="12.75">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" ht="12.75">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="12.75">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" ht="12.75">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="12.75">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -544,43 +640,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <printOptions/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
-  <sheetData/>
-  <printOptions/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.28125" widthPt="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="2.28125" widthPt="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="3.28125" widthPt="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="2.28125" widthPt="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75">
@@ -588,7 +655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:7" ht="12.75">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -610,31 +677,13 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="21" ht="12.75">
       <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="12.75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="12.75">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -656,31 +705,13 @@
       <c r="G22" t="s">
         <v>7</v>
       </c>
-      <c r="H22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" t="s">
-        <v>12</v>
-      </c>
-      <c r="M22" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="41" ht="12.75">
       <c r="A41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="12.75">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="12.75">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -702,31 +733,13 @@
       <c r="G42" t="s">
         <v>7</v>
       </c>
-      <c r="H42" t="s">
-        <v>8</v>
-      </c>
-      <c r="I42" t="s">
-        <v>9</v>
-      </c>
-      <c r="J42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K42" t="s">
-        <v>11</v>
-      </c>
-      <c r="L42" t="s">
-        <v>12</v>
-      </c>
-      <c r="M42" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="61" ht="12.75">
       <c r="A61" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="12.75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="12.75">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -747,228 +760,6 @@
       </c>
       <c r="G62" t="s">
         <v>7</v>
-      </c>
-      <c r="H62" t="s">
-        <v>8</v>
-      </c>
-      <c r="I62" t="s">
-        <v>9</v>
-      </c>
-      <c r="J62" t="s">
-        <v>10</v>
-      </c>
-      <c r="K62" t="s">
-        <v>11</v>
-      </c>
-      <c r="L62" t="s">
-        <v>12</v>
-      </c>
-      <c r="M62" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M62"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultColWidthPt="48.75" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="10.28125" widthPt="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="2.28125" widthPt="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="3.28125" widthPt="17.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="12.75">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="12.75">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" ht="12.75">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="12.75">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" t="s">
-        <v>10</v>
-      </c>
-      <c r="K22" t="s">
-        <v>11</v>
-      </c>
-      <c r="L22" t="s">
-        <v>12</v>
-      </c>
-      <c r="M22" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" ht="12.75">
-      <c r="A41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="12.75">
-      <c r="A42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
-        <v>5</v>
-      </c>
-      <c r="F42" t="s">
-        <v>6</v>
-      </c>
-      <c r="G42" t="s">
-        <v>7</v>
-      </c>
-      <c r="H42" t="s">
-        <v>8</v>
-      </c>
-      <c r="I42" t="s">
-        <v>9</v>
-      </c>
-      <c r="J42" t="s">
-        <v>10</v>
-      </c>
-      <c r="K42" t="s">
-        <v>11</v>
-      </c>
-      <c r="L42" t="s">
-        <v>12</v>
-      </c>
-      <c r="M42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="61" ht="12.75">
-      <c r="A61" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="12.75">
-      <c r="A62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" t="s">
-        <v>2</v>
-      </c>
-      <c r="C62" t="s">
-        <v>3</v>
-      </c>
-      <c r="D62" t="s">
-        <v>4</v>
-      </c>
-      <c r="E62" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" t="s">
-        <v>6</v>
-      </c>
-      <c r="G62" t="s">
-        <v>7</v>
-      </c>
-      <c r="H62" t="s">
-        <v>8</v>
-      </c>
-      <c r="I62" t="s">
-        <v>9</v>
-      </c>
-      <c r="J62" t="s">
-        <v>10</v>
-      </c>
-      <c r="K62" t="s">
-        <v>11</v>
-      </c>
-      <c r="L62" t="s">
-        <v>12</v>
-      </c>
-      <c r="M62" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>